<commit_message>
Take how much Excel sucks and multiply it by a thousand and you might get in the ballpark of how bad libreoffice is
</commit_message>
<xml_diff>
--- a/assign4/data.xlsx
+++ b/assign4/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>Algorithm</t>
   </si>
@@ -28,10 +28,16 @@
     <t>Avg. time (ms.)</t>
   </si>
   <si>
-    <t>Avg. moves (ms)</t>
+    <t>Avg. moves</t>
   </si>
   <si>
     <t>basic</t>
+  </si>
+  <si>
+    <t>greedy</t>
+  </si>
+  <si>
+    <t>random</t>
   </si>
 </sst>
 </file>
@@ -131,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B19" activeCellId="0" pane="topLeft" sqref="B19"/>
+      <selection activeCell="F10" activeCellId="0" pane="topLeft" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -324,6 +330,336 @@
       </c>
       <c r="D13" s="0" t="n">
         <v>124.9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2.029</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>8.3333</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>72.282</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>71.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>213.587</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>278.011</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>53.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>751.173</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>82.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1209.045</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1969.064</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3435.527</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>110.6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>3874.541</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>91.6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>5889.61</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>104.2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>8539.096</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>115.9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>10362.746</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>111.4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2.597</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>56.955</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>59.4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>284.025</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>118.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>824.94</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1835.517</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>210.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2739.308</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>194.4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>3096.128</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>146.888</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>5885.65</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>193.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>10157.307</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>241.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>11259.35</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>205.2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>13663.043</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>186.571</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New picture and data
</commit_message>
<xml_diff>
--- a/assign4/data.xlsx
+++ b/assign4/data.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="8">
   <si>
     <t>Algorithm</t>
   </si>
@@ -43,12 +43,15 @@
   <si>
     <t>random</t>
   </si>
+  <si>
+    <t>awesome</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -57,6 +60,20 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -78,15 +95,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -217,6 +238,15 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$13</c:f>
@@ -1579,6 +1609,346 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0776523177618761"/>
+          <c:y val="0.0397310513447433"/>
+          <c:w val="0.724934794709954"/>
+          <c:h val="0.812510347881331"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. moves</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$38:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>117.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="25"/>
+        <c:axId val="2086805496"/>
+        <c:axId val="2086887128"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. time (ms.)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.872</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>353.578</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664.871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1434.128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1627.986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3200.174</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3909.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5704.808</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7484.402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10870.556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2075494728"/>
+        <c:axId val="2086760392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2086805496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Queens</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086887128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2086887128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg. Moves</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086805496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2086760392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg. Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2075494728"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2075494728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086760392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88185968629634"/>
+          <c:y val="0.350506805536838"/>
+          <c:w val="0.105312491582794"/>
+          <c:h val="0.298986388926323"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1700,6 +2070,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>264160</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2030,10 +2432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AC22" sqref="AC22"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2561,9 +2963,177 @@
         <v>248.88800000000001</v>
       </c>
     </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2">
+        <v>102.872</v>
+      </c>
+      <c r="D39" s="2">
+        <v>101.88800000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2">
+        <v>15</v>
+      </c>
+      <c r="C40" s="2">
+        <v>142.619</v>
+      </c>
+      <c r="D40" s="2">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2">
+        <v>20</v>
+      </c>
+      <c r="C41" s="2">
+        <v>353.57799999999997</v>
+      </c>
+      <c r="D41" s="2">
+        <v>69.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2">
+        <v>25</v>
+      </c>
+      <c r="C42" s="2">
+        <v>664.87099999999998</v>
+      </c>
+      <c r="D42" s="2">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="2">
+        <v>30</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1434.1279999999999</v>
+      </c>
+      <c r="D43" s="2">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2">
+        <v>35</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1627.9860000000001</v>
+      </c>
+      <c r="D44" s="2">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2">
+        <v>40</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3200.174</v>
+      </c>
+      <c r="D45" s="2">
+        <v>104.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3909.54</v>
+      </c>
+      <c r="D46" s="2">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="2">
+        <v>50</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5704.808</v>
+      </c>
+      <c r="D47" s="2">
+        <v>102.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="2">
+        <v>55</v>
+      </c>
+      <c r="C48" s="2">
+        <v>7484.402</v>
+      </c>
+      <c r="D48" s="2">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="2">
+        <v>60</v>
+      </c>
+      <c r="C49" s="2">
+        <v>10870.556</v>
+      </c>
+      <c r="D49" s="2">
+        <v>117.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
another graph over to other computer
</commit_message>
<xml_diff>
--- a/assign4/data.xlsx
+++ b/assign4/data.xlsx
@@ -1949,6 +1949,366 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>awesome</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.872</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>353.578</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664.871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1434.128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1627.986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3200.174</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3909.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5704.808</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7484.402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10870.556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>213.587</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>278.011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>751.173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1209.045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1969.064</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3435.527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3874.541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5889.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8539.096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10362.746</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2110484264"/>
+        <c:axId val="2110314968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2110484264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of Queens</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2110314968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2110314968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2110484264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2102,6 +2462,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>820420</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2434,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="L79" workbookViewId="0">
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
data for the naiive restarting feature
</commit_message>
<xml_diff>
--- a/assign4/data.xlsx
+++ b/assign4/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
   <si>
     <t>Algorithm</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>awesome</t>
+  </si>
+  <si>
+    <t>restarts</t>
   </si>
 </sst>
 </file>
@@ -95,8 +98,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -105,9 +112,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2309,6 +2320,366 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>restarts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.406</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>381.243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>817.714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1309.012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001.062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2702.452</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4820.891</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6344.487</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9848.529</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10539.942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>213.587</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>278.011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>751.173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1209.045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1969.064</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3435.527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3874.541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5889.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8539.096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10362.746</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2108056200"/>
+        <c:axId val="2063511240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2108056200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of Queens</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2063511240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2063511240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2108056200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2494,6 +2865,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>820420</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2824,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L79" workbookViewId="0">
-      <selection activeCell="Q89" sqref="Q89"/>
+    <sheetView tabSelected="1" topLeftCell="P109" workbookViewId="0">
+      <selection activeCell="Q118" sqref="Q118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3521,6 +3924,174 @@
       </c>
       <c r="D49" s="2">
         <v>117.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="2">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2.4060000000000001</v>
+      </c>
+      <c r="D50" s="2">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="2">
+        <v>10</v>
+      </c>
+      <c r="C51" s="2">
+        <v>138.95099999999999</v>
+      </c>
+      <c r="D51" s="2">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="2">
+        <v>15</v>
+      </c>
+      <c r="C52" s="2">
+        <v>149.05600000000001</v>
+      </c>
+      <c r="D52" s="2">
+        <v>57.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="2">
+        <v>20</v>
+      </c>
+      <c r="C53" s="2">
+        <v>381.24299999999999</v>
+      </c>
+      <c r="D53" s="2">
+        <v>59.33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="2">
+        <v>25</v>
+      </c>
+      <c r="C54" s="2">
+        <v>817.71400000000006</v>
+      </c>
+      <c r="D54" s="2">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="2">
+        <v>30</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1309.0119999999999</v>
+      </c>
+      <c r="D55" s="2">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="2">
+        <v>35</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2001.0619999999999</v>
+      </c>
+      <c r="D56" s="2">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="2">
+        <v>40</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2702.4520000000002</v>
+      </c>
+      <c r="D57" s="2">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="2">
+        <v>45</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4820.8909999999996</v>
+      </c>
+      <c r="D58" s="2">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="2">
+        <v>50</v>
+      </c>
+      <c r="C59" s="2">
+        <v>6344.4870000000001</v>
+      </c>
+      <c r="D59" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="2">
+        <v>55</v>
+      </c>
+      <c r="C60" s="2">
+        <v>9848.5290000000005</v>
+      </c>
+      <c r="D60" s="2">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="2">
+        <v>60</v>
+      </c>
+      <c r="C61" s="2">
+        <v>10539.941999999999</v>
+      </c>
+      <c r="D61" s="2">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>